<commit_message>
Fixed feature labels in charts
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Saturn-Dashboard.xlsx
+++ b/blueprint-jira-better-excel/Saturn-Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{C6113708-CAB3-490A-8C36-7B7629FA23D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:180000_{EC4DDA48-A638-4BB6-B292-7163694D1D27}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   </definedNames>
   <calcPr calcId="179017"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId19"/>
+    <pivotCache cacheId="15" r:id="rId19"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -1922,7 +1922,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="0" baseline="0"/>
-              <a:t>CPM Progress</a:t>
+              <a:t>Reuse Progress</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="0"/>
           </a:p>
@@ -2128,7 +2128,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>CPM Progress</a:t>
+              <a:t>Reuse Progress</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2570,7 +2570,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CPM Backlog by State</a:t>
+              <a:t>Reuse Backlog by State</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3576,7 +3576,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>CPM Burndown</a:t>
+              <a:t>Reuse Burndown</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3998,7 +3998,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CPM Cumulative Flow Diagram</a:t>
+              <a:t>Reuse Cumulative Flow Diagram</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5033,7 +5033,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="0" baseline="0"/>
-              <a:t>Excel Import Progress</a:t>
+              <a:t>Drag &amp; Drop Progress</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="0"/>
           </a:p>
@@ -5241,7 +5241,7 @@
               <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Excel Import</a:t>
+              <a:t>Drag &amp; Drop</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -5687,7 +5687,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Excel Import Backlog by State</a:t>
+              <a:t>Drag &amp; Drop Backlog by State</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -6702,7 +6702,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Excel Import Burndown</a:t>
+              <a:t>Drag &amp; Drop Burndown</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -7334,11 +7334,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Excel</a:t>
+              <a:t>Drag</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Import</a:t>
+              <a:t> &amp; Drop</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -8336,7 +8336,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="0" baseline="0"/>
-              <a:t>UME v2 Progress</a:t>
+              <a:t>UME v3 Progress</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="0"/>
           </a:p>
@@ -8542,7 +8542,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>UME v2 Progress</a:t>
+              <a:t>UME v3 Progress</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -8980,7 +8980,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>UME v2 Burndown</a:t>
+              <a:t>UME v3 Burndown</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -9406,7 +9406,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> v2</a:t>
+              <a:t> v3</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US"/>
@@ -10243,7 +10243,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> v2 Backlog by State</a:t>
+              <a:t> v3 Backlog by State</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -42609,7 +42609,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43486.693218865737" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="104" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43487.623498148147" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="104" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -42905,8 +42905,8 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Saturn Component" numFmtId="0">
-      <sharedItems containsBlank="1" count="9">
-        <s v="${bpHelper.getRocketComponent(issue)}"/>
+      <sharedItems containsBlank="1" count="10">
+        <s v="${bpHelper.getSaturnComponent(issue)}"/>
         <m/>
         <s v="UME v3"/>
         <s v="Reuse"/>
@@ -42915,6 +42915,7 @@
         <s v="R&amp;D Bucket"/>
         <s v="Other"/>
         <s v="CI/CD"/>
+        <s v="${bpHelper.getRocketComponent(issue)}" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Customer" numFmtId="0">
@@ -48098,8 +48099,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -48195,7 +48196,7 @@
   <pageFields count="3">
     <pageField fld="32" item="5" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="2" hier="-1"/>
+    <pageField fld="10" item="7" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
@@ -48213,8 +48214,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
-  <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
+  <location ref="G29:H34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -48335,7 +48336,7 @@
   <pageFields count="4">
     <pageField fld="32" item="5" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="7" hier="-1"/>
+    <pageField fld="10" item="8" hier="-1"/>
     <pageField fld="45" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="5">
@@ -48345,7 +48346,7 @@
     <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
     <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
   </dataFields>
-  <chartFormats count="21">
+  <chartFormats count="27">
     <chartFormat chart="0" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="2">
@@ -48487,7 +48488,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="9" format="19" series="1">
+    <chartFormat chart="7" format="7" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -48496,7 +48497,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="9" format="20">
+    <chartFormat chart="7" format="8">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -48505,7 +48506,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="9" format="21">
+    <chartFormat chart="7" format="9">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -48514,7 +48515,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="9" format="22">
+    <chartFormat chart="7" format="10">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -48523,7 +48524,7 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="9" format="23">
+    <chartFormat chart="7" format="11">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -48532,7 +48533,61 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="9" format="24">
+    <chartFormat chart="7" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="24">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -48555,8 +48610,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -48580,28 +48635,41 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item m="1" x="6"/>
+        <item x="4"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item m="1" x="8"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" showAll="0">
       <items count="7">
         <item x="0"/>
@@ -48614,14 +48682,14 @@
       </items>
     </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
@@ -48635,187 +48703,49 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="-2"/>
+    <field x="10"/>
   </rowFields>
   <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <pageFields count="3">
     <pageField fld="32" item="5" hier="-1"/>
     <pageField fld="1" hier="-1"/>
     <pageField fld="45" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
   </dataFields>
-  <chartFormats count="15">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -48829,7 +48759,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AL10:AP17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -48987,7 +48917,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49093,7 +49023,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G5:H8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField showAll="0"/>
@@ -49217,7 +49147,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A6:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49457,7 +49387,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B5:C12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49699,7 +49629,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D5:E14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49999,7 +49929,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="B29:C36" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -50272,7 +50202,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B9:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -50694,7 +50624,1362 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="44"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Story Points" fld="13" baseField="44" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="18">
+    <chartFormat chart="2" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+  <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item m="1" x="6"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item m="1" x="8"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="32" item="5" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="7" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="21">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A54:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="35"/>
+  </rowFields>
+  <rowItems count="8">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="1" item="2" hier="-1"/>
+    <pageField fld="32" item="5" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="2" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="5" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="15">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="5" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item m="1" x="6"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item m="1" x="8"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="7">
+        <item x="0"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="5" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="J29:K34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51143,1027 +52428,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
-  <location ref="G29:H34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item m="1" x="6"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="4">
-    <pageField fld="32" item="5" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="8" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
-  </dataFields>
-  <chartFormats count="27">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="44"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Story Points" fld="13" baseField="44" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="18">
-    <chartFormat chart="2" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A54:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="35"/>
-  </rowFields>
-  <rowItems count="8">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="1" item="2" hier="-1"/>
-    <pageField fld="32" item="5" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="2" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="5" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="15" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="G41:G42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -52261,270 +52527,6 @@
     <pageField fld="32" item="5" hier="-1"/>
     <pageField fld="1" hier="-1"/>
     <pageField fld="10" item="8" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="1"/>
-        <item m="1" x="6"/>
-        <item x="4"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="5" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="31" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item m="1" x="6"/>
-        <item x="4"/>
-        <item x="1"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item m="1" x="8"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="7">
-        <item x="0"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="5" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="7" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
@@ -58359,13 +58361,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.46484375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -58729,7 +58731,7 @@
       </c>
       <c r="E6" s="25">
         <f ca="1">TODAY()</f>
-        <v>43486</v>
+        <v>43487</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>264</v>

</xml_diff>